<commit_message>
Darkest before the dawn
</commit_message>
<xml_diff>
--- a/excel/Test1.xlsx
+++ b/excel/Test1.xlsx
@@ -482,6 +482,10 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <f>C10+Sheet2!A2</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -491,12 +495,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Changed a lot of things, added better dependency tracking
</commit_message>
<xml_diff>
--- a/excel/Test1.xlsx
+++ b/excel/Test1.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28702"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaxw/SunshineFart3000/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="120" windowWidth="19008" windowHeight="9360"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="24680" windowHeight="15080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +111,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -144,12 +162,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -176,14 +194,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -210,6 +229,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,26 +405,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.8" customHeight="1">
+    <row r="2" spans="1:5" ht="31.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -412,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -421,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" thickTop="1" thickBot="1">
+    <row r="4" spans="1:5" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>A2+A3</f>
         <v>3</v>
@@ -434,12 +454,12 @@
         <v>turd3borderpoop33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickTop="1">
+    <row r="5" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -448,7 +468,7 @@
         <v>turd 12&amp; border12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -457,7 +477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -472,7 +492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -494,26 +514,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -524,13 +542,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f>Sheet1!A2+Sheet1!E10</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>